<commit_message>
Project Macro Risk 2020-02-12
</commit_message>
<xml_diff>
--- a/HH_Projects/02_Macro_Risk/Data_Files/Source_Files/Ratings_Scale.xlsx
+++ b/HH_Projects/02_Macro_Risk/Data_Files/Source_Files/Ratings_Scale.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Job\GitHub Repository\HH_Codebase\HH_Projects\02_Macro_Risk\Data_Files\Source_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6716EDD-8AEF-4584-A835-2688A798F0DA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AA3949-F2F7-40FC-AC1B-669291E5E0E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E870CE67-903F-4A44-88B0-74FF9AA40FEC}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E870CE67-903F-4A44-88B0-74FF9AA40FEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Scale Comparision" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -535,9 +536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C358018A-20CD-45BC-9D90-140B8B07FC88}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>